<commit_message>
update data fill in to string for export
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/CombingBillingByJob.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/CombingBillingByJob.xlsx
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
   <si>
     <t>INDO TRANS LOGISTICS CORPORATION</t>
   </si>
@@ -142,9 +142,6 @@
     <t>Hóa Đơn/Invoice</t>
   </si>
   <si>
-    <t xml:space="preserve">Tổng cộng/Total (VND) </t>
-  </si>
-  <si>
     <t>{SOANo}</t>
   </si>
   <si>
@@ -199,9 +196,6 @@
     <t>{CusAuthTotal}</t>
   </si>
   <si>
-    <t>{FrieghtInvoice}</t>
-  </si>
-  <si>
     <t>{FreightFee}</t>
   </si>
   <si>
@@ -224,6 +218,45 @@
   </si>
   <si>
     <t>{CombineNo}</t>
+  </si>
+  <si>
+    <t>{FrieghtOBHInvoice}</t>
+  </si>
+  <si>
+    <t>{CusFeeTotal}</t>
+  </si>
+  <si>
+    <t>{CusVATTotal}</t>
+  </si>
+  <si>
+    <t>{CusSumTotal}</t>
+  </si>
+  <si>
+    <t>{AuthFeeTotal}</t>
+  </si>
+  <si>
+    <t>{AuthVATTotal}</t>
+  </si>
+  <si>
+    <t>{AuthSumTotal}</t>
+  </si>
+  <si>
+    <t>{CusAuthSumTotal}</t>
+  </si>
+  <si>
+    <t>{FreFeeTotal}</t>
+  </si>
+  <si>
+    <t>{FreVATTotal}</t>
+  </si>
+  <si>
+    <t>{FreSumTotal}</t>
+  </si>
+  <si>
+    <t>{PTSumTotal}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{LabelTotal} </t>
   </si>
 </sst>
 </file>
@@ -600,7 +633,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -694,6 +727,80 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="37" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="37" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="37" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -708,75 +815,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="37" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="37" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="37" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="37" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="37" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="37" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="37" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="37" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="37" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="37" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -1124,14 +1162,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11:U13"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="40" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
@@ -1139,7 +1177,7 @@
     <col min="7" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="16.5703125" customWidth="1"/>
     <col min="10" max="16" width="20" style="16" customWidth="1"/>
-    <col min="17" max="17" width="18.42578125" customWidth="1"/>
+    <col min="17" max="17" width="35.7109375" customWidth="1"/>
     <col min="18" max="18" width="12.42578125" style="16" customWidth="1"/>
     <col min="19" max="19" width="13" style="16" customWidth="1"/>
     <col min="20" max="20" width="20" style="16" customWidth="1"/>
@@ -1155,197 +1193,197 @@
     </row>
     <row r="2" spans="1:23" ht="50.1" customHeight="1">
       <c r="L2" s="17"/>
-      <c r="M2" s="43" t="s">
+      <c r="M2" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="23"/>
       <c r="S2" s="23"/>
       <c r="T2" s="23"/>
     </row>
     <row r="4" spans="1:23" ht="20.25">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="44"/>
-      <c r="N4" s="44"/>
-      <c r="O4" s="44"/>
-      <c r="P4" s="44"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="72"/>
+      <c r="M4" s="72"/>
+      <c r="N4" s="72"/>
+      <c r="O4" s="72"/>
+      <c r="P4" s="72"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="24"/>
       <c r="S4" s="24"/>
       <c r="T4" s="24"/>
     </row>
     <row r="5" spans="1:23" ht="18.75">
-      <c r="A5" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="46"/>
+      <c r="A5" s="73" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="74"/>
+      <c r="P5" s="74"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="25"/>
       <c r="S5" s="25"/>
       <c r="T5" s="25"/>
     </row>
     <row r="6" spans="1:23" ht="19.5">
-      <c r="A6" s="47" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="47"/>
-      <c r="P6" s="47"/>
+      <c r="A6" s="75" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="75"/>
+      <c r="N6" s="75"/>
+      <c r="O6" s="75"/>
+      <c r="P6" s="75"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="26"/>
       <c r="S6" s="26"/>
       <c r="T6" s="26"/>
     </row>
     <row r="7" spans="1:23" ht="19.5">
-      <c r="A7" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="47"/>
-      <c r="O7" s="47"/>
-      <c r="P7" s="47"/>
+      <c r="A7" s="75" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
       <c r="Q7" s="7"/>
       <c r="R7" s="26"/>
       <c r="S7" s="26"/>
       <c r="T7" s="26"/>
     </row>
     <row r="8" spans="1:23" ht="13.5" thickBot="1">
-      <c r="A8" s="62" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="62"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="62"/>
-      <c r="N8" s="62"/>
-      <c r="O8" s="62"/>
-      <c r="P8" s="62"/>
+      <c r="A8" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="54"/>
+      <c r="P8" s="54"/>
       <c r="Q8" s="8"/>
       <c r="R8" s="27"/>
       <c r="S8" s="27"/>
       <c r="T8" s="27"/>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="36.75" customHeight="1">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="56" t="s">
+      <c r="C9" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="56" t="s">
+      <c r="D9" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="56" t="s">
+      <c r="E9" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="56" t="s">
+      <c r="F9" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="56" t="s">
+      <c r="G9" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="63" t="s">
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="63"/>
-      <c r="L9" s="63"/>
-      <c r="M9" s="63" t="s">
+      <c r="K9" s="56"/>
+      <c r="L9" s="56"/>
+      <c r="M9" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="N9" s="63"/>
-      <c r="O9" s="63"/>
-      <c r="P9" s="64" t="s">
+      <c r="N9" s="56"/>
+      <c r="O9" s="56"/>
+      <c r="P9" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="Q9" s="51" t="s">
+      <c r="Q9" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="R9" s="52"/>
-      <c r="S9" s="52"/>
-      <c r="T9" s="53"/>
-      <c r="U9" s="60" t="s">
+      <c r="R9" s="64"/>
+      <c r="S9" s="64"/>
+      <c r="T9" s="65"/>
+      <c r="U9" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="V9" s="48" t="s">
+      <c r="V9" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="W9" s="50" t="s">
+      <c r="W9" s="62" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="36.75" customHeight="1">
-      <c r="A10" s="59"/>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
+      <c r="A10" s="69"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
       <c r="G10" s="2" t="s">
         <v>17</v>
       </c>
@@ -1373,7 +1411,7 @@
       <c r="O10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="P10" s="61"/>
+      <c r="P10" s="58"/>
       <c r="Q10" s="12" t="s">
         <v>22</v>
       </c>
@@ -1386,79 +1424,79 @@
       <c r="T10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="U10" s="61"/>
-      <c r="V10" s="49"/>
-      <c r="W10" s="50"/>
+      <c r="U10" s="58"/>
+      <c r="V10" s="61"/>
+      <c r="W10" s="62"/>
     </row>
     <row r="11" spans="1:23" s="3" customFormat="1" ht="16.5" customHeight="1">
       <c r="A11" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="C11" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="D11" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="E11" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="37" t="s">
+      <c r="F11" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="G11" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="40" t="s">
+      <c r="I11" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="L11" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="M11" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="N11" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="O11" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="P11" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q11" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="H11" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="J11" s="65" t="s">
-        <v>36</v>
-      </c>
-      <c r="K11" s="65" t="s">
-        <v>37</v>
-      </c>
-      <c r="L11" s="65" t="s">
-        <v>35</v>
-      </c>
-      <c r="M11" s="65" t="s">
-        <v>38</v>
-      </c>
-      <c r="N11" s="65" t="s">
-        <v>39</v>
-      </c>
-      <c r="O11" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="P11" s="66" t="s">
+      <c r="R11" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="Q11" s="67" t="s">
+      <c r="S11" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="R11" s="68" t="s">
+      <c r="T11" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="S11" s="68" t="s">
+      <c r="U11" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="T11" s="65" t="s">
+      <c r="V11" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="U11" s="66" t="s">
-        <v>46</v>
-      </c>
-      <c r="V11" s="38" t="s">
-        <v>47</v>
-      </c>
       <c r="W11" s="39" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:23" s="3" customFormat="1" ht="15.75" customHeight="1">
@@ -1471,80 +1509,66 @@
       <c r="G12" s="42"/>
       <c r="H12" s="30"/>
       <c r="I12" s="32"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
-      <c r="M12" s="69"/>
-      <c r="N12" s="69"/>
-      <c r="O12" s="69"/>
-      <c r="P12" s="70"/>
-      <c r="Q12" s="71"/>
-      <c r="R12" s="72"/>
-      <c r="S12" s="72"/>
-      <c r="T12" s="73"/>
-      <c r="U12" s="70"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="52"/>
+      <c r="S12" s="52"/>
+      <c r="T12" s="53"/>
+      <c r="U12" s="49"/>
       <c r="V12" s="15"/>
       <c r="W12" s="14"/>
     </row>
     <row r="13" spans="1:23" s="1" customFormat="1" ht="36" customHeight="1" thickBot="1">
-      <c r="A13" s="54" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="74">
-        <f>SUM(J11:J12)</f>
-        <v>0</v>
-      </c>
-      <c r="K13" s="74">
-        <f t="shared" ref="K13:U13" si="0">SUM(K11:K12)</f>
-        <v>0</v>
-      </c>
-      <c r="L13" s="74">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M13" s="74">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N13" s="74">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="74">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="74">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="74">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R13" s="74">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S13" s="74">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T13" s="74">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="U13" s="74">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="A13" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="67"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="K13" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="L13" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="M13" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="N13" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="O13" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="P13" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q13" s="44"/>
+      <c r="R13" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="S13" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="T13" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="U13" s="50" t="s">
+        <v>60</v>
       </c>
       <c r="V13" s="13"/>
       <c r="W13" s="13"/>
@@ -1594,13 +1618,11 @@
     <filterColumn colId="11" showButton="0"/>
   </autoFilter>
   <mergeCells count="21">
-    <mergeCell ref="A8:P8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="A4:P4"/>
+    <mergeCell ref="A5:P5"/>
+    <mergeCell ref="A6:P6"/>
+    <mergeCell ref="A7:P7"/>
     <mergeCell ref="V9:V10"/>
     <mergeCell ref="W9:W10"/>
     <mergeCell ref="Q9:T9"/>
@@ -1610,11 +1632,13 @@
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="U9:U10"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="A4:P4"/>
-    <mergeCell ref="A5:P5"/>
-    <mergeCell ref="A6:P6"/>
-    <mergeCell ref="A7:P7"/>
+    <mergeCell ref="A8:P8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>